<commit_message>
added different BSS methods experimantation
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shaig\Documents\CS_Technion\2019_b\Deep Learning Project\DL_project_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB10543-F575-4CA7-84A8-EC0EEBBE753A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96CE2333-D9BF-4E43-BED6-C1D2FE89D209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="12" windowWidth="23040" windowHeight="12348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>SHAI:</t>
   </si>
@@ -43,6 +44,9 @@
   </si>
   <si>
     <t>waiting</t>
+  </si>
+  <si>
+    <t>Try to run PCA or ICA before doing source seperation</t>
   </si>
 </sst>
 </file>
@@ -369,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,6 +409,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>